<commit_message>
fixed BOM line item
</commit_message>
<xml_diff>
--- a/modules/rf_spectrum/rev_b/rf_spectrum_bom.xlsx
+++ b/modules/rf_spectrum/rev_b/rf_spectrum_bom.xlsx
@@ -439,22 +439,22 @@
     <t xml:space="preserve">R4</t>
   </si>
   <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
     <t xml:space="preserve">311-100KLRCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-07100KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100k</t>
   </si>
   <si>
     <t xml:space="preserve">R7</t>
@@ -1549,21 +1549,21 @@
         <v>129</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>131</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>127</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>127</v>
@@ -1601,13 +1601,13 @@
         <v>129</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>131</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1615,7 +1615,7 @@
         <v>145</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>127</v>
@@ -1627,13 +1627,13 @@
         <v>129</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>131</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,7 +1641,7 @@
         <v>146</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>127</v>
@@ -1653,13 +1653,13 @@
         <v>129</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>131</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,7 +1667,7 @@
         <v>147</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>148</v>

</xml_diff>